<commit_message>
INDEV: Request Message Dto Created
New and modified dto list.
 - SQLTableDto
   - SQLTableColumnDto
 - SQLIndexesDto
   - SQLIndexDto
 - SQLConstraintsDto
   - SQLConsConstraintDto

extres/SQLBuilder_MessageSpec
- Wrong speling changed.
</commit_message>
<xml_diff>
--- a/extres/SQLBuilder_MessageSpec.xlsx
+++ b/extres/SQLBuilder_MessageSpec.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shud8\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\broadDev\sqlscriptbuilder\extres\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20925" windowHeight="9945" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20925" windowHeight="9945" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Changelog" sheetId="3" r:id="rId1"/>
@@ -58,9 +58,6 @@
     <t>originOwner</t>
   </si>
   <si>
-    <t>addtionalCommand</t>
-  </si>
-  <si>
     <t>synonym</t>
   </si>
   <si>
@@ -242,6 +239,10 @@
   </si>
   <si>
     <t>ArrayList</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>additionalCommand</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -773,7 +774,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
@@ -788,36 +789,36 @@
   <sheetData>
     <row r="2" spans="2:6">
       <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
         <v>35</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>36</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>37</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>38</v>
-      </c>
-      <c r="F2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" s="2">
         <v>44555</v>
       </c>
       <c r="D3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" t="s">
         <v>41</v>
-      </c>
-      <c r="E3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -830,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:S46"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -857,7 +858,7 @@
   <sheetData>
     <row r="3" spans="2:19">
       <c r="B3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -868,7 +869,7 @@
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -881,60 +882,60 @@
     </row>
     <row r="4" spans="2:19">
       <c r="B4" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="K4" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="Q4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="R4" s="3" t="s">
+      <c r="S4" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="5" spans="2:19">
       <c r="B5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -942,16 +943,16 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
@@ -961,45 +962,45 @@
     </row>
     <row r="6" spans="2:19">
       <c r="B6" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="2:19">
       <c r="B7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="2:19">
       <c r="B8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="2:19">
       <c r="C9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="2:19">
       <c r="C10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="2:19">
@@ -1007,7 +1008,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="2:19">
@@ -1015,7 +1016,7 @@
         <v>3</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="2:19">
@@ -1023,7 +1024,7 @@
         <v>8</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="2:19">
@@ -1031,7 +1032,7 @@
         <v>6</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="2:19">
@@ -1039,34 +1040,34 @@
         <v>1</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="2:19">
       <c r="D16" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="2:10">
       <c r="D17" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="2:10">
       <c r="D18" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="2:10">
@@ -1074,34 +1075,34 @@
         <v>2</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="2:10">
       <c r="B20" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="2:10">
       <c r="C21" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="2:10">
       <c r="C22" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="2:10">
@@ -1109,23 +1110,23 @@
         <v>5</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="2:10">
       <c r="D24" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="2:10">
       <c r="D25" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="2:10">
@@ -1133,7 +1134,7 @@
         <v>6</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="2:10">
@@ -1141,21 +1142,21 @@
         <v>8</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="2:10">
       <c r="D28" s="1" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="2:10">
@@ -1163,23 +1164,23 @@
         <v>9</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="2:10">
       <c r="C30" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="2:10">
       <c r="C31" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="2:10">
@@ -1187,7 +1188,7 @@
         <v>3</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="2:10">
@@ -1195,15 +1196,15 @@
         <v>7</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="2:10">
       <c r="D34" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="2:10">
@@ -1211,10 +1212,10 @@
         <v>6</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="2:10">
@@ -1222,18 +1223,18 @@
         <v>8</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="2:10">
       <c r="B37" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="2:10">
@@ -1241,7 +1242,7 @@
         <v>4</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="2:10">
@@ -1249,42 +1250,42 @@
         <v>11</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="2:10">
       <c r="C40" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="41" spans="2:10">
       <c r="B41" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="42" spans="2:10">
       <c r="C42" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="2:10">
       <c r="C43" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="2:10">
@@ -1297,18 +1298,18 @@
         <v>0</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="46" spans="2:10">
       <c r="D46" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>